<commit_message>
Created test cases to achieve branch and statement coverage
</commit_message>
<xml_diff>
--- a/branch_&_statement_coverage.xlsx
+++ b/branch_&_statement_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbste\Desktop\github\scholarship-eligibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{711D9354-9C1D-4AAF-9B53-B6A67330B7AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B27688-2EFC-4DA9-8FA3-FA93716B5663}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DD39A81-DC4D-4DF4-B627-D50BEA6774C6}"/>
   </bookViews>
@@ -30,6 +30,113 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="34">
+  <si>
+    <t>Paths</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Statements</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>a, b, f, l, s</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>a, c, d, f, l, s</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>a, c, e, g, i, l, s</t>
+  </si>
+  <si>
+    <t>a, c, e, h, k, m, o</t>
+  </si>
+  <si>
+    <t>a, c, e, g, j, k, m, p, q, s</t>
+  </si>
+  <si>
+    <t>a, c, e, h, k, m, p, r, t</t>
+  </si>
+  <si>
+    <t>a, c, e, h, k, n, t</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -49,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -57,12 +164,244 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +716,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66162D1A-BE5B-4621-B52E-104B7C5811F5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="28" width="4.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="13"/>
+    </row>
+    <row r="2" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10">
+        <v>4</v>
+      </c>
+      <c r="E2" s="10">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10">
+        <v>6</v>
+      </c>
+      <c r="G2" s="10">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="8"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="8"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="8"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="8"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="8"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC8" s="8"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC9" s="8"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A10" s="18"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:AB1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created test cases that achieve statement and branch coverage
</commit_message>
<xml_diff>
--- a/branch_&_statement_coverage.xlsx
+++ b/branch_&_statement_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbste\Desktop\github\scholarship-eligibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B27688-2EFC-4DA9-8FA3-FA93716B5663}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25988E9-BA8C-42EA-B3CB-C7F44988B50B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DD39A81-DC4D-4DF4-B627-D50BEA6774C6}"/>
   </bookViews>
@@ -719,7 +719,7 @@
   <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added expected outputs to table
</commit_message>
<xml_diff>
--- a/branch_&_statement_coverage.xlsx
+++ b/branch_&_statement_coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbste\Desktop\github\scholarship-eligibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25988E9-BA8C-42EA-B3CB-C7F44988B50B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCD6241-60A6-4108-A311-922F85327CAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3DD39A81-DC4D-4DF4-B627-D50BEA6774C6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="36">
   <si>
     <t>Paths</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>a, c, e, h, k, n, t</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>D. F. C</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -354,11 +360,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,15 +444,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,6 +453,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66162D1A-BE5B-4621-B52E-104B7C5811F5}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,43 +803,46 @@
     <col min="2" max="28" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="11" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="13"/>
-    </row>
-    <row r="2" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -846,12 +924,14 @@
       <c r="AA2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="13"/>
+    </row>
+    <row r="3" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -893,10 +973,13 @@
         <v>26</v>
       </c>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="8"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="AC3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="8"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -942,10 +1025,13 @@
         <v>26</v>
       </c>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="8"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="AC4" s="19">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="8"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -997,10 +1083,13 @@
         <v>26</v>
       </c>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="8"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="AC5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="8"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1054,10 +1143,13 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="8"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="AC6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD6" s="8"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1121,10 +1213,13 @@
         <v>26</v>
       </c>
       <c r="AB7" s="5"/>
-      <c r="AC7" s="8"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="AC7" s="23">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="8"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1184,10 +1279,13 @@
       <c r="AB8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC8" s="8"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+      <c r="AC8" s="19">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="8"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1239,44 +1337,49 @@
       <c r="AB9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC9" s="8"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
+      <c r="AC9" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="8"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="AC10" s="15"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:AB1"/>
+    <mergeCell ref="AC1:AC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>